<commit_message>
Changes to upload instructions based on updated tool
</commit_message>
<xml_diff>
--- a/static/documents/GeneralResourceUploadTemplate.xlsx
+++ b/static/documents/GeneralResourceUploadTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdpearso\Documents\GitHub\BioKIC\symbiota-docs\static\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A681D7-9E29-436A-856F-65EB03D3E47B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE40E61-CD56-4FCA-A70C-D1EE87E3DCFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="9060" activeTab="1" xr2:uid="{02916371-48DD-48A1-875F-97ECF4093F61}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>resourceUrl</t>
   </si>
@@ -37,30 +37,12 @@
     <t>establishedDate</t>
   </si>
   <si>
-    <t>identifier</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
-    <t>objectOccurrenceID</t>
-  </si>
-  <si>
-    <t>objectCatalogNumber</t>
-  </si>
-  <si>
-    <t>objectOccid</t>
-  </si>
-  <si>
     <t>relationshipID</t>
   </si>
   <si>
-    <t>subType</t>
-  </si>
-  <si>
-    <t>verbatimSciname</t>
-  </si>
-  <si>
     <t>subjectOccurrenceID</t>
   </si>
   <si>
@@ -127,37 +109,37 @@
     <t>The date when the relationship between the subject and the object was asserted.</t>
   </si>
   <si>
-    <t>A string used to identify the object record that it is not its catalog number or occurrenceID. For reference only, not used to link directly to the external or internal resource.</t>
-  </si>
-  <si>
     <t>Comments about the relationship between the subject and the object.</t>
   </si>
   <si>
-    <t>The primary human-readable identifier for the object record you are linking to the subject.</t>
-  </si>
-  <si>
-    <t>The global unique identifier (GUID) of the object record you are linking to the subject.</t>
-  </si>
-  <si>
     <t>https://dwc.tdwg.org/terms/#dwc:relationshipRemarks</t>
   </si>
   <si>
     <t>https://dwc.tdwg.org/terms/#dwc:catalogNumber</t>
   </si>
   <si>
-    <t>The occid (internal Symbiota reference number) for the object record you are linking to the subject.</t>
-  </si>
-  <si>
     <t>An identifier for the relationship type that connects the subject to its object.</t>
   </si>
   <si>
     <t>https://dwc.tdwg.org/terms/#dwc:relationshipOfResourceID</t>
   </si>
   <si>
-    <t>A relationship type that falls hierarchically beneath the selected relationship type.</t>
-  </si>
-  <si>
-    <t>The taxonomic name of the object of the association/relationship.</t>
+    <t>according to</t>
+  </si>
+  <si>
+    <t>The source (person, organization, publication, reference) establishing the relationship between the two resources.</t>
+  </si>
+  <si>
+    <t>https://dwc.tdwg.org/terms/#dwc:relationshipAccordingTo</t>
+  </si>
+  <si>
+    <t>objectID</t>
+  </si>
+  <si>
+    <t>https://dwc.tdwg.org/terms/#dwc:relatedResourceID</t>
+  </si>
+  <si>
+    <t>An identifier for a related resource (the object, rather than the subject of the relationship).</t>
   </si>
 </sst>
 </file>
@@ -256,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -277,6 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,87 +574,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05B8B9-35CD-4411-A1E3-08DC9A76B0A3}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="17" style="7" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" style="7" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -680,10 +642,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFD9393-3F0C-4F13-9008-5329CF2A5AFB}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,197 +658,153 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2</v>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>